<commit_message>
multivariate model for two outcomes need to add power prior
</commit_message>
<xml_diff>
--- a/02_data/pda_outcomes.xlsx
+++ b/02_data/pda_outcomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheTimbot\Dropbox\School\PhD\pda_dec_tool\02_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE5DA24-B76B-49B3-B226-2F0248D8ED44}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA642DF-D21F-4643-BEF5-F7F026031D16}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10065" firstSheet="1" activeTab="7" xr2:uid="{C85B0458-FC89-4B11-8D7C-C4EF5E18DBD2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10065" firstSheet="1" activeTab="4" xr2:uid="{C85B0458-FC89-4B11-8D7C-C4EF5E18DBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="closure" sheetId="1" r:id="rId1"/>
@@ -211,84 +211,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -8368,7 +8291,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12 B2:E11">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>B2="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10936,7 +10859,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12 B2:E11">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>B2="NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15472,8 +15395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF45FC89-6BD2-4A92-8B9B-DED463A19259}">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15611,7 +15534,7 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S2">
         <v>8</v>
@@ -25344,8 +25267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42A94F-DE12-4BEB-AE07-93DCF152A103}">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>